<commit_message>
feat(migration): deploy in prod and ROI. Done
</commit_message>
<xml_diff>
--- a/Annexes/[Annexe 1] Map competences - projects.xlsx
+++ b/Annexes/[Annexe 1] Map competences - projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julien/Documents/Mes Documents/Mémoire/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376650FB-A63E-8E45-ACF8-5E794D3ADBAB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA5AE06-D30D-7045-B51E-1A43EB551797}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{180DDFB3-D36C-6248-B464-0E2671F73A5A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>Compétence</t>
   </si>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70847723-DBE4-1F44-ABB2-40B976A63AB1}">
   <dimension ref="B2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1"/>
@@ -1019,7 +1019,9 @@
       <c r="D27" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="10"/>
+      <c r="E27" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="2:5" ht="40" customHeight="1">
       <c r="B28" s="6" t="s">
@@ -1041,7 +1043,9 @@
       <c r="D29" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="10"/>
+      <c r="E29" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="2:5" ht="40" customHeight="1">
       <c r="B30" s="8" t="s">
@@ -1063,7 +1067,9 @@
       <c r="D31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="10"/>
+      <c r="E31" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="2:5" ht="40" customHeight="1">
       <c r="B32" s="8" t="s">

</xml_diff>